<commit_message>
Working on Help section
</commit_message>
<xml_diff>
--- a/website/flask/static/forms/analysis_submission_form.xlsx
+++ b/website/flask/static/forms/analysis_submission_form.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="6460" yWindow="1040" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Analysis Title</t>
   </si>
@@ -216,17 +216,47 @@
     <t>Metadata</t>
   </si>
   <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Recommended</t>
+    <t>Associated Objects</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Enrichment analysis of genes upregulated in prostate cancer</t>
+  </si>
+  <si>
+    <t>Core Elements</t>
+  </si>
+  <si>
+    <t>An enrichment analysis was performed on the top 500 most overexpressed genes determined by comparing prostate cancer samples to normal samples.</t>
+  </si>
+  <si>
+    <t>http://amp.pharm.mssm.edu/Enrichr/enrich?dataset=2p28v</t>
+  </si>
+  <si>
+    <t>GSE3468</t>
+  </si>
+  <si>
+    <t>Enrichr</t>
+  </si>
+  <si>
+    <t>enrichment
+prostate cancer
+upregulated</t>
+  </si>
+  <si>
+    <t>geneset: upregulated
+disease: prostate cancer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,30 +265,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
@@ -269,8 +275,51 @@
       <color indexed="81"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +338,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -298,25 +353,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -592,59 +676,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="7" customWidth="1"/>
+    <col min="4" max="7" width="22.6640625" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="3">
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added icons, working on upload form
</commit_message>
<xml_diff>
--- a/website/flask/static/forms/analysis_submission_form.xlsx
+++ b/website/flask/static/forms/analysis_submission_form.xlsx
@@ -188,12 +188,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Denis Torre:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Preview image for the analysis.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Analysis Title</t>
   </si>
@@ -250,13 +272,22 @@
   <si>
     <t>geneset: upregulated
 disease: prostate cancer</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Preview URL</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/denis-torre/datasets2tools-canned-analyses/master/data/screenshots/Enrichr/Enrichr%20Dn%203.png?raw=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -318,8 +349,31 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +398,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -368,22 +428,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -397,6 +461,26 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -676,82 +760,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" style="7" customWidth="1"/>
-    <col min="4" max="7" width="22.6640625" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="22.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="4" customWidth="1"/>
+    <col min="4" max="7" width="22.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>